<commit_message>
update single value template
</commit_message>
<xml_diff>
--- a/template/Checklist-golive-{TABLE_NAME}.xlsx
+++ b/template/Checklist-golive-{TABLE_NAME}.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\24122023\08.FBNK_SEAB_CR_GIFT_IMPORT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\19122023\01.FBNK_SEAB_SALARY_CUSTOMER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A0D1E-15E6-4683-B078-EF1B8D22ACAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B667F0C-D876-4E80-8BE0-E72BCB0C0801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCOUNT(INIT)" sheetId="9" state="hidden" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="137">
   <si>
     <t>No</t>
   </si>
@@ -293,6 +293,9 @@
     <t>Set thuộc tính parsing cho trường multi</t>
   </si>
   <si>
+    <t>Không set</t>
+  </si>
+  <si>
     <t>2. Tạo stream INIT</t>
   </si>
   <si>
@@ -379,97 +382,77 @@
 Kiểm tra những trường cần string join để cắt theo đúng delimiter đã chọn</t>
   </si>
   <si>
-    <t>Nếu đã có topic MAPPED từ trước, kiểm tra message xem đã được đánh index
- '- Nếu có, bỏ qua bước 4.2
-'- Nếu chưa có, thực hiện bước 4.2</t>
-  </si>
-  <si>
-    <t>set 'ksql.functions._global_.xml.parser.add.multivalue.index'='true';</t>
-  </si>
-  <si>
-    <t>Insert schema vào bảng STANDARD_MANUAL nếu chưa có schema trên Confluent</t>
-  </si>
-  <si>
-    <t>Nếu bảng multi đi từ bảng Single, bỏ qua bước tạo topic và stream gốc</t>
-  </si>
-  <si>
-    <t>Checklist golive ODS_SEAB_CR_GIFT_IMPORT</t>
+    <t>Checklist golive ODS_SEAB_SALARY_CUSTOMER</t>
   </si>
   <si>
     <t>Lệnh check:
-curl -X GET http://&lt;schema_registry_IP&gt;:8081/subjects/MAP_SS_FBNK_SEAB_CR_GIFT_IMPORT-value/versions/1</t>
-  </si>
-  <si>
-    <t>MAP_SS_FBNK_SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_INIT</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_INIT_MAPPED</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_INIT_MULTIVALUE</t>
-  </si>
-  <si>
-    <t>ODS_SEAB_CR_GIFT_IMPORT_INIT</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_MAPPED</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_MULTIVALUE</t>
-  </si>
-  <si>
-    <t>ODS_SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>Tạo bảng ODS_SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa bảng ODS_SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>0.1 FBNK_SEAB_CR_GIFT_IMPORT_v0.1</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_MAPPED_v0.1.sql</t>
-  </si>
-  <si>
-    <t>ODS_SEAB_CR_GIFT_IMPORT_v0.1.sql</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_INIT_v0.1.sql</t>
-  </si>
-  <si>
-    <t>FBNK_SEAB_CR_GIFT_IMPORT_INIT_MAPPED_v0.1</t>
-  </si>
-  <si>
-    <t>ODS_SEAB_CR_GIFT_IMPORT_INIT_v0.1</t>
-  </si>
-  <si>
-    <t>connector_T_SEAB_CR_GIFT_IMPORT2Ods_config</t>
-  </si>
-  <si>
-    <t>connector_T_SEAB_CR_GIFT_IMPORT2Ods_config_init</t>
-  </si>
-  <si>
-    <t>Thêm vào luồng &lt;EXTRACT_NAME&gt; để capture dữ liệu từ bảng SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>Thêm vào luồng &lt;REPLICAT_NAME&gt; để đẩy dữ liệu lên trên topic FBNK_SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>Tạo luồng &lt;EXTRACT_INIT_NAME&gt; để init dữ liệu từ bảng SEAB_CR_GIFT_IMPORT</t>
-  </si>
-  <si>
-    <t>Thêm vào luồng &lt;REPLICAT_INIT_NAME&gt; để đẩy dữ liệu lên trên topic FBNK_SEAB_CR_GIFT_IMPORT_INIT</t>
-  </si>
-  <si>
-    <t>SEAB_CR_GÌT_IMPORT_DDL_v0.1</t>
+curl -X GET http://&lt;schema_registry_IP&gt;:8081/subjects/MAP_SS_FBNK_SEAB_SALARY_CUSTOMER-value/versions/1</t>
+  </si>
+  <si>
+    <t>MAP_SS_FBNK_SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER_INIT</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER_INIT_MAPPED</t>
+  </si>
+  <si>
+    <t>ODS_SEAB_SALARY_CUSTOMER_INIT</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER_MAPPED</t>
+  </si>
+  <si>
+    <t>ODS_SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>Tạo bảng ODS_SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>D:\haidn\CHECKLIST_GOLIVE\01. SEAB_SALARY_CUSTOMER\01. DDL</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa bảng ODS_SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>0.1 FBNK_SEAB_SALARY_CUSTOMER_v0.1</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER_MAPPED_v0.1.sql</t>
+  </si>
+  <si>
+    <t>ODS_SEAB_SALARY_CUSTOMER_v0.1.sql</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER_INIT_v0.1.sql</t>
+  </si>
+  <si>
+    <t>FBNK_SEAB_SALARY_CUSTOMER_INIT_MAPPED_v0.1</t>
+  </si>
+  <si>
+    <t>ODS_SEAB_SALARY_CUSTOMER_INIT_v0.1</t>
+  </si>
+  <si>
+    <t>connector_T_SEAB_SALARY_CUSTOMER2Ods_config</t>
+  </si>
+  <si>
+    <t>connector_T_SEAB_SALARY_CUSTOMER2Ods_config_init</t>
+  </si>
+  <si>
+    <t>Thêm vào luồng &lt;EXTRACT_NAME&gt; để capture dữ liệu từ bảng SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>Thêm vào luồng &lt;REPLICAT_NAME&gt; để đẩy dữ liệu lên trên topic FBNK_SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>Tạo luồng &lt;EXTRACT_INIT_NAME&gt; để init dữ liệu từ bảng SEAB_SALARY_CUSTOMER</t>
+  </si>
+  <si>
+    <t>Thêm vào luồng &lt;REPLICAT_INIT_NAME&gt; để đẩy dữ liệu lên trên topic FBNK_SEAB_SALARY_CUSTOMER_INIT</t>
   </si>
 </sst>
 </file>
@@ -683,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -766,56 +749,41 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1153,20 +1121,20 @@
       <selection activeCell="A13" sqref="A13:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>64</v>
       </c>
@@ -1178,7 +1146,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +1184,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>47</v>
@@ -1236,7 +1204,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>22</v>
@@ -1258,7 +1226,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
@@ -1270,7 +1238,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1292,7 +1260,7 @@
       </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1314,7 +1282,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -1336,7 +1304,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -1358,7 +1326,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -1380,7 +1348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1360,7 @@
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>6</v>
       </c>
@@ -1416,7 +1384,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>7</v>
       </c>
@@ -1438,7 +1406,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>8</v>
       </c>
@@ -1462,7 +1430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>9</v>
       </c>
@@ -1484,7 +1452,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>18</v>
       </c>
@@ -1496,7 +1464,7 @@
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>9</v>
       </c>
@@ -1518,7 +1486,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>10</v>
       </c>
@@ -1538,7 +1506,7 @@
       </c>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>11</v>
       </c>
@@ -1558,7 +1526,7 @@
       </c>
       <c r="H20" s="22"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>12</v>
       </c>
@@ -1593,102 +1561,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:L27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="44.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="62.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="61.5546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="68" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="44.5703125" style="10"/>
+    <col min="13" max="16384" width="44.5546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="48"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+        <v>87</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>94</v>
-      </c>
       <c r="I3" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K3" s="17"/>
       <c r="L3" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="11" t="s">
         <v>70</v>
       </c>
@@ -1702,15 +1670,15 @@
       <c r="K4" s="11"/>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="11" t="s">
         <v>69</v>
       </c>
@@ -1723,203 +1691,215 @@
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+    </row>
+    <row r="7" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>1</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="12">
+        <v>16</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="C12" s="12">
+        <v>16</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="28"/>
+      <c r="L12" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>4</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>5</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-    </row>
-    <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="B13" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="12">
+        <v>16</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
         <v>1</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>1</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="B15" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="C14" s="12">
-        <v>16</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>2</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>120</v>
       </c>
       <c r="C15" s="12">
         <v>16</v>
@@ -1927,7 +1907,9 @@
       <c r="D15" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="30"/>
+      <c r="E15" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="F15" s="11"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -1935,17 +1917,19 @@
       <c r="J15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="30"/>
+      <c r="K15" s="28" t="s">
+        <v>74</v>
+      </c>
       <c r="L15" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="12">
         <v>16</v>
@@ -1953,21 +1937,25 @@
       <c r="D16" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="30"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="11"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="13"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="28"/>
+      <c r="L16" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="12">
         <v>16</v>
@@ -1975,7 +1963,7 @@
       <c r="D17" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="30"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="11"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -1983,71 +1971,55 @@
       <c r="J17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="30"/>
+      <c r="K17" s="28"/>
       <c r="L17" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+    </row>
+    <row r="19" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
         <v>1</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B20" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="12">
-        <v>16</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>2</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" s="12">
-        <v>16</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="30"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
@@ -2055,221 +2027,229 @@
       <c r="J20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K20" s="11"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" s="12">
-        <v>16</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="30"/>
+        <v>124</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="30"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>4</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" s="12">
-        <v>16</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="30"/>
-      <c r="L22" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-    </row>
-    <row r="24" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+    <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+    </row>
+    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
         <v>1</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="13"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>2</v>
-      </c>
       <c r="B26" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="11" t="s">
-        <v>71</v>
+        <v>119</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-    </row>
-    <row r="28" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="J26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>2</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="35"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
+        <v>3</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="28"/>
+      <c r="L28" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
+        <v>4</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="28"/>
+      <c r="L29" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+    </row>
+    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>1</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="37"/>
+      <c r="E31" s="28" t="s">
         <v>72</v>
       </c>
       <c r="F31" s="11"/>
@@ -2279,45 +2259,45 @@
       <c r="J31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="30" t="s">
-        <v>74</v>
+      <c r="K31" s="38" t="s">
+        <v>102</v>
       </c>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>2</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="30"/>
+      <c r="C32" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="28"/>
       <c r="F32" s="11"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
       <c r="J32" s="11"/>
-      <c r="K32" s="30"/>
+      <c r="K32" s="38"/>
       <c r="L32" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>3</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
+        <v>117</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="28"/>
       <c r="F33" s="11"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
@@ -2325,83 +2305,91 @@
       <c r="J33" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K33" s="30"/>
+      <c r="K33" s="38"/>
       <c r="L33" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>4</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="30"/>
+        <v>118</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="33"/>
+      <c r="E34" s="28"/>
       <c r="F34" s="11"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
-        <v>5</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="J34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="38"/>
+      <c r="L34" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+    </row>
+    <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
+        <v>1</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K35" s="30"/>
-      <c r="L35" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D36" s="33"/>
+      <c r="E36" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="30" t="s">
-        <v>72</v>
-      </c>
+      <c r="D37" s="33"/>
+      <c r="E37" s="28"/>
       <c r="F37" s="11"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
@@ -2409,87 +2397,79 @@
       <c r="J37" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K37" s="41" t="s">
+      <c r="K37" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+    </row>
+    <row r="39" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="L37" s="12"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
-        <v>2</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="36"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
-        <v>3</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39" s="29" t="s">
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+    </row>
+    <row r="40" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="11">
+        <v>1</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K39" s="41"/>
-      <c r="L39" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
-        <v>4</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="30"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="F40" s="11"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="12"/>
-    </row>
-    <row r="41" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="J40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="L40" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="28"/>
       <c r="F41" s="11"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
@@ -2497,41 +2477,39 @@
       <c r="J41" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K41" s="41"/>
-      <c r="L41" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K41" s="28"/>
+      <c r="L41" s="38"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="11">
+        <v>3</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="28"/>
+      <c r="L42" s="38"/>
+    </row>
+    <row r="43" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30" t="s">
-        <v>75</v>
-      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="28"/>
       <c r="F43" s="11"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
@@ -2539,25 +2517,21 @@
       <c r="J43" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="K43" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="L43" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L43" s="38"/>
+    </row>
+    <row r="44" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="28"/>
       <c r="F44" s="11"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
@@ -2565,233 +2539,86 @@
       <c r="J44" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K44" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-    </row>
-    <row r="46" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="37"/>
-      <c r="L46" s="37"/>
-    </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
-        <v>1</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K47" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="L47" s="41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
-        <v>2</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K48" s="30"/>
-      <c r="L48" s="41"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
-        <v>3</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K49" s="30"/>
-      <c r="L49" s="41"/>
-    </row>
-    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
-        <v>4</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K50" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="L50" s="41"/>
-    </row>
-    <row r="51" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
-        <v>5</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K51" s="30"/>
-      <c r="L51" s="41"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
+      <c r="K44" s="28"/>
+      <c r="L44" s="38"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="11">
         <v>6</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B45" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K52" s="30"/>
-      <c r="L52" s="41"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K45" s="28"/>
+      <c r="L45" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="B7:D7"/>
+  <mergeCells count="44">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="L40:L45"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="K26:K29"/>
+    <mergeCell ref="K31:K34"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E40:E45"/>
+    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="K43:K45"/>
+    <mergeCell ref="E26:E29"/>
     <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="K19:K22"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="L47:L52"/>
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="K31:K35"/>
-    <mergeCell ref="K37:K41"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="K47:K49"/>
-    <mergeCell ref="K50:K52"/>
-    <mergeCell ref="E31:E35"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="A38:L38"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C25:D25" r:id="rId1" display="Z:\2. Noi bo Team\5.VAN HANH ETL STREAMING\01. Golive T24SB\01. ACCOUNT\01. DDL\ACCOUNT_DDL_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C31:D31" r:id="rId2" display="FBNK_ACCOUNT_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C33:D33" r:id="rId3" display="FBNK_ACCOUNT_MAPPED_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C35:D35" r:id="rId4" display="ODS_ACCOUNT_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="C37:D37" r:id="rId5" display="FBNK_ACCOUNT_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="C39:D39" r:id="rId6" display="FBNK_ACCOUNT_INIT_MAPPED_v0.1" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="C41:D41" r:id="rId7" display="ODS_ACCOUNT_INIT_v0.1" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="C43:D43" r:id="rId8" display="connector_T_Account2Ods_config" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="C44:D44" r:id="rId9" display="connector_T_Account2Ods_config_init" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="C20:D20" r:id="rId1" display="Z:\2. Noi bo Team\5.VAN HANH ETL STREAMING\01. Golive T24SB\01. ACCOUNT\01. DDL\ACCOUNT_DDL_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C26:D26" r:id="rId2" display="FBNK_ACCOUNT_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C28:D28" r:id="rId3" display="FBNK_ACCOUNT_MAPPED_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C29:D29" r:id="rId4" display="ODS_ACCOUNT_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C31:D31" r:id="rId5" display="FBNK_ACCOUNT_v0.1.sql" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C33:D33" r:id="rId6" display="FBNK_ACCOUNT_INIT_MAPPED_v0.1" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C34:D34" r:id="rId7" display="ODS_ACCOUNT_INIT_v0.1" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="C36:D36" r:id="rId8" display="connector_T_Account2Ods_config" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="C37:D37" r:id="rId9" display="connector_T_Account2Ods_config_init" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -2806,20 +2633,20 @@
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="40" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="53.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="53.109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>65</v>
       </c>
@@ -2831,7 +2658,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2857,7 +2684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>21</v>
       </c>
@@ -2869,7 +2696,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="5" t="s">
         <v>28</v>
@@ -2889,7 +2716,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5" t="s">
         <v>22</v>
@@ -2911,19 +2738,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -2945,7 +2772,7 @@
       </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -2967,7 +2794,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -2987,7 +2814,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -3009,7 +2836,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -3031,7 +2858,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -3053,7 +2880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>17</v>
       </c>
@@ -3065,7 +2892,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>7</v>
       </c>
@@ -3089,7 +2916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>8</v>
       </c>
@@ -3113,7 +2940,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>9</v>
       </c>
@@ -3137,7 +2964,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>10</v>
       </c>
@@ -3161,7 +2988,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>11</v>
       </c>
@@ -3183,7 +3010,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>18</v>
       </c>
@@ -3195,7 +3022,7 @@
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>12</v>
       </c>
@@ -3217,7 +3044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>13</v>
       </c>
@@ -3237,7 +3064,7 @@
       </c>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>14</v>
       </c>
@@ -3257,7 +3084,7 @@
       </c>
       <c r="H22" s="22"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>15</v>
       </c>

</xml_diff>